<commit_message>
Schedule tables updated and reset synchronized. Still not running Noc_test.java in the FPGA.
</commit_message>
<xml_diff>
--- a/noc/results/results.xlsx
+++ b/noc/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="20925" windowHeight="10590"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="18870" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>Resources pr. tile</t>
   </si>
@@ -72,12 +72,6 @@
     <t>Fmax</t>
   </si>
   <si>
-    <t>Router [MHz]</t>
-  </si>
-  <si>
-    <t>Tile [MHz]</t>
-  </si>
-  <si>
     <t>Period length</t>
   </si>
   <si>
@@ -112,6 +106,15 @@
   </si>
   <si>
     <t>Period</t>
+  </si>
+  <si>
+    <t>Router (MHz)</t>
+  </si>
+  <si>
+    <t>Tile (MHz)</t>
+  </si>
+  <si>
+    <t>New measurement</t>
   </si>
 </sst>
 </file>
@@ -249,6 +252,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -275,18 +290,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -360,7 +363,7 @@
                   <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>222</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>340</c:v>
@@ -436,7 +439,7 @@
                   <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>147</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>205</c:v>
@@ -740,7 +743,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>26</c:v>
@@ -914,18 +917,18 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="174109824"/>
-        <c:axId val="174111360"/>
+        <c:axId val="59382784"/>
+        <c:axId val="59396864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174109824"/>
+        <c:axId val="59382784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="Standard" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174111360"/>
+        <c:crossAx val="59396864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -933,7 +936,7 @@
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174111360"/>
+        <c:axId val="59396864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,7 +944,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="Standard" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174109824"/>
+        <c:crossAx val="59382784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
@@ -956,7 +959,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1284,13 +1287,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -1304,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
         <v>17</v>
@@ -1313,50 +1315,50 @@
     <row r="2" spans="1:21" ht="15.75" thickBot="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="M2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
       <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>27</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>28</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" t="s">
-        <v>30</v>
       </c>
       <c r="S2" t="s">
         <v>12</v>
@@ -1365,14 +1367,14 @@
         <v>13</v>
       </c>
       <c r="U2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="10">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1382,25 +1384,25 @@
         <v>86</v>
       </c>
       <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
         <v>44</v>
-      </c>
-      <c r="F3" s="2">
-        <v>4</v>
       </c>
       <c r="G3" s="2">
         <v>4</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="10">
         <v>5</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="11">
         <v>207</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="11">
         <v>103</v>
       </c>
-      <c r="K3" s="12" t="s">
-        <v>22</v>
+      <c r="K3" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="M3">
         <f>B3</f>
@@ -1419,15 +1421,15 @@
         <v>0.25600000000000001</v>
       </c>
       <c r="Q3">
+        <f>F3</f>
+        <v>44</v>
+      </c>
+      <c r="R3">
+        <f>F4</f>
+        <v>100</v>
+      </c>
+      <c r="S3">
         <f>E3</f>
-        <v>44</v>
-      </c>
-      <c r="R3">
-        <f>E4</f>
-        <v>100</v>
-      </c>
-      <c r="S3">
-        <f>F3</f>
         <v>4</v>
       </c>
       <c r="T3">
@@ -1440,23 +1442,23 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="16"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1">
         <v>64</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
         <v>100</v>
       </c>
-      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="13"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="17"/>
       <c r="M4">
         <f>B6</f>
         <v>9</v>
@@ -1474,15 +1476,15 @@
         <v>0.51200000000000001</v>
       </c>
       <c r="Q4">
+        <f>F6</f>
+        <v>71</v>
+      </c>
+      <c r="R4">
+        <f>F7</f>
+        <v>103</v>
+      </c>
+      <c r="S4">
         <f>E6</f>
-        <v>71</v>
-      </c>
-      <c r="R4">
-        <f>E7</f>
-        <v>103</v>
-      </c>
-      <c r="S4">
-        <f>F6</f>
         <v>6</v>
       </c>
       <c r="T4">
@@ -1495,8 +1497,8 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1506,37 +1508,37 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="14"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="18"/>
       <c r="M5">
         <f>B9</f>
         <v>16</v>
       </c>
       <c r="N5">
         <f>D9</f>
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="O5">
         <f>D10</f>
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="P5">
         <f>D11/1000</f>
         <v>1.024</v>
       </c>
       <c r="Q5">
+        <f>F9</f>
+        <v>89</v>
+      </c>
+      <c r="R5">
+        <f>F10</f>
+        <v>105</v>
+      </c>
+      <c r="S5">
         <f>E9</f>
-        <v>89</v>
-      </c>
-      <c r="R5">
-        <f>E10</f>
-        <v>105</v>
-      </c>
-      <c r="S5">
-        <f>F9</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="T5">
         <f>G9</f>
@@ -1548,10 +1550,10 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="10">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1561,24 +1563,24 @@
         <v>159</v>
       </c>
       <c r="E6" s="5">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5">
         <v>71</v>
-      </c>
-      <c r="F6" s="5">
-        <v>6</v>
       </c>
       <c r="G6" s="5">
         <v>7</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="10">
         <v>10</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="10">
         <v>183</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="10">
         <v>97</v>
       </c>
-      <c r="K6" s="9"/>
+      <c r="K6" s="13"/>
       <c r="M6">
         <f>B12</f>
         <v>25</v>
@@ -1596,15 +1598,15 @@
         <v>1.024</v>
       </c>
       <c r="Q6">
+        <f>F12</f>
+        <v>98</v>
+      </c>
+      <c r="R6">
+        <f>F13</f>
+        <v>106</v>
+      </c>
+      <c r="S6">
         <f>E12</f>
-        <v>98</v>
-      </c>
-      <c r="R6">
-        <f>E13</f>
-        <v>106</v>
-      </c>
-      <c r="S6">
-        <f>F12</f>
         <v>26</v>
       </c>
       <c r="T6">
@@ -1617,23 +1619,23 @@
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="16"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="1">
         <v>104</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
         <v>103</v>
       </c>
-      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="14"/>
       <c r="M7">
         <f>B15</f>
         <v>36</v>
@@ -1651,15 +1653,15 @@
         <v>2.048</v>
       </c>
       <c r="Q7">
+        <f>F15</f>
+        <v>99</v>
+      </c>
+      <c r="R7">
+        <f>F16</f>
+        <v>107</v>
+      </c>
+      <c r="S7">
         <f>E15</f>
-        <v>99</v>
-      </c>
-      <c r="R7">
-        <f>E16</f>
-        <v>107</v>
-      </c>
-      <c r="S7">
-        <f>F15</f>
         <v>52</v>
       </c>
       <c r="T7">
@@ -1672,8 +1674,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1683,10 +1685,10 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="15"/>
       <c r="M8">
         <f>B18</f>
         <v>49</v>
@@ -1704,15 +1706,15 @@
         <v>2.048</v>
       </c>
       <c r="Q8">
+        <f>F18</f>
+        <v>99</v>
+      </c>
+      <c r="R8">
+        <f>F19</f>
+        <v>107</v>
+      </c>
+      <c r="S8">
         <f>E18</f>
-        <v>99</v>
-      </c>
-      <c r="R8">
-        <f>E19</f>
-        <v>107</v>
-      </c>
-      <c r="S8">
-        <f>F18</f>
         <v>73</v>
       </c>
       <c r="T8">
@@ -1725,37 +1727,39 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="10">
         <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="5">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E9" s="5">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5">
         <v>89</v>
-      </c>
-      <c r="F9" s="5">
-        <v>18</v>
       </c>
       <c r="G9" s="5">
         <v>19</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="10">
         <v>19</v>
       </c>
-      <c r="I9" s="6">
-        <v>150</v>
-      </c>
-      <c r="J9" s="6">
-        <v>100</v>
-      </c>
-      <c r="K9" s="9"/>
+      <c r="I9" s="10">
+        <v>206</v>
+      </c>
+      <c r="J9" s="10">
+        <v>96</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="M9">
         <f>B21</f>
         <v>64</v>
@@ -1773,15 +1777,15 @@
         <v>2.048</v>
       </c>
       <c r="Q9">
+        <f>F21</f>
+        <v>100</v>
+      </c>
+      <c r="R9">
+        <f>F22</f>
+        <v>108</v>
+      </c>
+      <c r="S9">
         <f>E21</f>
-        <v>100</v>
-      </c>
-      <c r="R9">
-        <f>E22</f>
-        <v>108</v>
-      </c>
-      <c r="S9">
-        <f>F21</f>
         <v>111</v>
       </c>
       <c r="T9">
@@ -1794,23 +1798,23 @@
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="16"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="1">
-        <v>147</v>
-      </c>
-      <c r="E10" s="1">
+        <v>139</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
         <v>105</v>
       </c>
-      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="14"/>
       <c r="M10">
         <f>B24</f>
         <v>81</v>
@@ -1828,15 +1832,15 @@
         <v>4.0960000000000001</v>
       </c>
       <c r="Q10">
+        <f>F24</f>
+        <v>100</v>
+      </c>
+      <c r="R10">
+        <f>F25</f>
+        <v>108</v>
+      </c>
+      <c r="S10">
         <f>E24</f>
-        <v>100</v>
-      </c>
-      <c r="R10">
-        <f>E25</f>
-        <v>108</v>
-      </c>
-      <c r="S10">
-        <f>F24</f>
         <v>167</v>
       </c>
       <c r="T10">
@@ -1849,8 +1853,8 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1860,16 +1864,16 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="11"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="10">
         <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1879,47 +1883,47 @@
         <v>340</v>
       </c>
       <c r="E12" s="5">
+        <v>26</v>
+      </c>
+      <c r="F12" s="5">
         <v>98</v>
-      </c>
-      <c r="F12" s="5">
-        <v>26</v>
       </c>
       <c r="G12" s="5">
         <v>22</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="10">
         <v>27</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="10">
         <v>154</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="10">
         <v>96</v>
       </c>
-      <c r="K12" s="9"/>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="16"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="1">
         <v>205</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
         <v>106</v>
       </c>
-      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A14" s="17"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1929,16 +1933,16 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="11"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="10">
         <v>36</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1948,47 +1952,47 @@
         <v>445</v>
       </c>
       <c r="E15" s="5">
+        <v>52</v>
+      </c>
+      <c r="F15" s="5">
         <v>99</v>
-      </c>
-      <c r="F15" s="5">
-        <v>52</v>
       </c>
       <c r="G15" s="5">
         <v>37</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="10">
         <v>42</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="10">
         <v>138</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="10">
         <v>101</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="16"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="1">
         <v>276</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
         <v>107</v>
       </c>
-      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A17" s="17"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1998,16 +2002,16 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="11"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="10">
         <v>49</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -2017,47 +2021,47 @@
         <v>627</v>
       </c>
       <c r="E18" s="5">
+        <v>73</v>
+      </c>
+      <c r="F18" s="5">
         <v>99</v>
-      </c>
-      <c r="F18" s="5">
-        <v>73</v>
       </c>
       <c r="G18" s="5">
         <v>50</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="10">
         <v>58</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="10">
         <v>128</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="10">
         <v>100</v>
       </c>
-      <c r="K18" s="9"/>
+      <c r="K18" s="13"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="16"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="1">
         <v>354</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
         <v>107</v>
       </c>
-      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A20" s="17"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
@@ -2067,16 +2071,16 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="11"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="10">
         <v>64</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -2086,49 +2090,49 @@
         <v>649</v>
       </c>
       <c r="E21" s="5">
+        <v>111</v>
+      </c>
+      <c r="F21" s="5">
         <v>100</v>
-      </c>
-      <c r="F21" s="5">
-        <v>111</v>
       </c>
       <c r="G21" s="5">
         <v>78</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="10">
         <v>87</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="10">
         <v>133</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="10">
         <v>101</v>
       </c>
-      <c r="K21" s="9" t="s">
-        <v>24</v>
+      <c r="K21" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="16"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="1">
         <v>445</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
         <v>108</v>
       </c>
-      <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="10"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A23" s="17"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="3" t="s">
         <v>15</v>
       </c>
@@ -2138,16 +2142,16 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="11"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="10">
         <v>81</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -2157,45 +2161,45 @@
         <v>812</v>
       </c>
       <c r="E24" s="5">
+        <v>167</v>
+      </c>
+      <c r="F24" s="5">
         <v>100</v>
-      </c>
-      <c r="F24" s="5">
-        <v>167</v>
       </c>
       <c r="G24" s="5">
         <v>121</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="10">
         <v>113</v>
       </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="9" t="s">
-        <v>25</v>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="16"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="1">
         <v>551</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1">
         <v>108</v>
       </c>
-      <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="10"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A26" s="17"/>
-      <c r="B26" s="8"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="3" t="s">
         <v>15</v>
       </c>
@@ -2205,16 +2209,16 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="11"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="10">
         <v>100</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -2224,16 +2228,16 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="6">
+      <c r="H27" s="10">
         <v>157</v>
       </c>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="9"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="13"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="16"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
@@ -2241,14 +2245,14 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="10"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A29" s="17"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="3" t="s">
         <v>15</v>
       </c>
@@ -2256,51 +2260,13 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="11"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="K21:K23"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="K24:K26"/>
     <mergeCell ref="K27:K29"/>
@@ -2317,6 +2283,44 @@
     <mergeCell ref="H27:H29"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="K6:K8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="K21:K23"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
New measurements added in Results.xlsx
</commit_message>
<xml_diff>
--- a/noc/results/results.xlsx
+++ b/noc/results/results.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="18870" windowHeight="10185"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="18870" windowHeight="10185" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
-    <sheet name="Ark2" sheetId="2" r:id="rId2"/>
-    <sheet name="Ark3" sheetId="3" r:id="rId3"/>
+    <sheet name="Diagram1" sheetId="4" r:id="rId1"/>
+    <sheet name="Ark1" sheetId="1" r:id="rId2"/>
+    <sheet name="Ark2" sheetId="2" r:id="rId3"/>
+    <sheet name="Ark3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>Resources pr. tile</t>
   </si>
@@ -84,12 +85,6 @@
     <t>Cores</t>
   </si>
   <si>
-    <t>Cyclon 3 chip</t>
-  </si>
-  <si>
-    <t>Did not fit in the Cyclon 3 chip</t>
-  </si>
-  <si>
     <t>NI:LUT</t>
   </si>
   <si>
@@ -115,16 +110,26 @@
   </si>
   <si>
     <t>New measurement</t>
+  </si>
+  <si>
+    <t>Did not fit in the Cyclon 2 chip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,25 +250,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -282,14 +274,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -306,18 +341,15 @@
   <c:chart>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>NI:LUT</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>'Ark1'!$M$3:$M$10</c:f>
               <c:numCache>
@@ -349,8 +381,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>'Ark1'!$N$3:$N$10</c:f>
               <c:numCache>
@@ -363,26 +395,27 @@
                   <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>227</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>340</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>445</c:v>
+                  <c:v>347</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>627</c:v>
+                  <c:v>449</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>649</c:v>
+                  <c:v>579</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>812</c:v>
+                  <c:v>771</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -390,10 +423,7 @@
           <c:tx>
             <c:v>NI:Reg</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>'Ark1'!$M$3:$M$10</c:f>
               <c:numCache>
@@ -425,8 +455,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>'Ark1'!$O$3:$O$10</c:f>
               <c:numCache>
@@ -439,26 +469,27 @@
                   <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>139</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>205</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>276</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>354</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>445</c:v>
+                  <c:v>307</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>551</c:v>
+                  <c:v>379</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -466,10 +497,7 @@
           <c:tx>
             <c:v>NI:Blockram</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>'Ark1'!$M$3:$M$10</c:f>
               <c:numCache>
@@ -501,8 +529,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>'Ark1'!$P$3:$P$10</c:f>
               <c:numCache>
@@ -515,7 +543,7 @@
                   <c:v>0.51200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.024</c:v>
+                  <c:v>0.51200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.024</c:v>
@@ -534,7 +562,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -542,10 +571,7 @@
           <c:tx>
             <c:v>Router:LUT</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>'Ark1'!$M$3:$M$10</c:f>
               <c:numCache>
@@ -577,8 +603,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>'Ark1'!$Q$3:$Q$10</c:f>
               <c:numCache>
@@ -591,26 +617,27 @@
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>99</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>181</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -618,10 +645,7 @@
           <c:tx>
             <c:v>Router:Reg</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>'Ark1'!$M$3:$M$10</c:f>
               <c:numCache>
@@ -653,8 +677,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>'Ark1'!$R$3:$R$10</c:f>
               <c:numCache>
@@ -686,18 +710,16 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="7"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>NI_ST</c:v>
+            <c:v>Period</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>'Ark1'!$M$3:$M$10</c:f>
               <c:numCache>
@@ -729,160 +751,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Ark1'!$S$3:$S$10</c:f>
-              <c:numCache>
-                <c:formatCode>Standard</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>111</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>167</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>Router_ST</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Ark1'!$M$3:$M$10</c:f>
-              <c:numCache>
-                <c:formatCode>Standard</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>81</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Ark1'!$T$3:$T$10</c:f>
-              <c:numCache>
-                <c:formatCode>Standard</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>121</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:v>Period</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Ark1'!$M$3:$M$10</c:f>
-              <c:numCache>
-                <c:formatCode>Standard</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>81</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>'Ark1'!$U$3:$U$10</c:f>
               <c:numCache>
@@ -914,29 +784,26 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="59382784"/>
-        <c:axId val="59396864"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="59382784"/>
+        <c:axId val="87264640"/>
+        <c:axId val="87274624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="87264640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="Standard" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59396864"/>
+        <c:crossAx val="87274624"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="59396864"/>
+        <c:axId val="87274624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -944,9 +811,9 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="Standard" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59382784"/>
+        <c:crossAx val="87264640"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
         <c:minorUnit val="20"/>
       </c:valAx>
@@ -957,33 +824,31 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9296937" cy="6063803"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagram 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -996,7 +861,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1288,7 +1153,7 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12:K14"/>
+      <selection activeCell="I9" sqref="I9:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1313,52 +1178,52 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="M2" t="s">
         <v>21</v>
       </c>
       <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>25</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>26</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" t="s">
-        <v>28</v>
       </c>
       <c r="S2" t="s">
         <v>12</v>
@@ -1367,41 +1232,41 @@
         <v>13</v>
       </c>
       <c r="U2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="15">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="16">
         <v>86</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="16">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="16">
         <v>44</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="16">
         <v>4</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="15">
         <v>5</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="17">
         <v>207</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="17">
         <v>103</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="18" t="s">
         <v>20</v>
       </c>
       <c r="M3">
@@ -1429,12 +1294,12 @@
         <v>100</v>
       </c>
       <c r="S3">
-        <f>E3</f>
-        <v>4</v>
+        <f>E3/H3*100</f>
+        <v>80</v>
       </c>
       <c r="T3">
-        <f>G3</f>
-        <v>4</v>
+        <f>G3/H3*100</f>
+        <v>80</v>
       </c>
       <c r="U3">
         <f>H3</f>
@@ -1442,23 +1307,23 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="7"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="1" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="20">
         <v>64</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
+      <c r="E4" s="20"/>
+      <c r="F4" s="20">
         <v>100</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="17"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="21"/>
       <c r="M4">
         <f>B6</f>
         <v>9</v>
@@ -1484,12 +1349,12 @@
         <v>103</v>
       </c>
       <c r="S4">
-        <f>E6</f>
-        <v>6</v>
+        <f>E6/H6*100</f>
+        <v>60</v>
       </c>
       <c r="T4">
-        <f>G6</f>
-        <v>7</v>
+        <f>G6/H6*100</f>
+        <v>70</v>
       </c>
       <c r="U4">
         <f>H6</f>
@@ -1497,52 +1362,52 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="24">
         <v>256</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="18"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="25"/>
       <c r="M5">
         <f>B9</f>
         <v>16</v>
       </c>
       <c r="N5">
         <f>D9</f>
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="O5">
         <f>D10</f>
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="P5">
         <f>D11/1000</f>
-        <v>1.024</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="Q5">
         <f>F9</f>
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="R5">
         <f>F10</f>
         <v>105</v>
       </c>
       <c r="S5">
-        <f>E9</f>
-        <v>19</v>
+        <f>E9/H9*100</f>
+        <v>94.73684210526315</v>
       </c>
       <c r="T5">
-        <f>G9</f>
-        <v>19</v>
+        <f>G9/H9*100</f>
+        <v>100</v>
       </c>
       <c r="U5">
         <f>H9</f>
@@ -1550,48 +1415,48 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="15">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="27">
         <v>159</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="27">
         <v>6</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="27">
         <v>71</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="27">
         <v>7</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="15">
         <v>10</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="15">
         <v>183</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="15">
         <v>97</v>
       </c>
-      <c r="K6" s="13"/>
+      <c r="K6" s="28"/>
       <c r="M6">
         <f>B12</f>
         <v>25</v>
       </c>
       <c r="N6">
         <f>D12</f>
-        <v>340</v>
+        <v>250</v>
       </c>
       <c r="O6">
         <f>D13</f>
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="P6">
         <f>D14/1000</f>
@@ -1599,19 +1464,19 @@
       </c>
       <c r="Q6">
         <f>F12</f>
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="R6">
         <f>F13</f>
         <v>106</v>
       </c>
       <c r="S6">
-        <f>E12</f>
-        <v>26</v>
+        <f>E12/H12*100</f>
+        <v>103.7037037037037</v>
       </c>
       <c r="T6">
-        <f>G12</f>
-        <v>22</v>
+        <f>G12/H12*100</f>
+        <v>85.18518518518519</v>
       </c>
       <c r="U6">
         <f>H12</f>
@@ -1619,34 +1484,34 @@
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="7"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="1" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="20">
         <v>104</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1">
+      <c r="E7" s="20"/>
+      <c r="F7" s="20">
         <v>103</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="14"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="29"/>
       <c r="M7">
         <f>B15</f>
         <v>36</v>
       </c>
       <c r="N7">
         <f>D15</f>
-        <v>445</v>
+        <v>347</v>
       </c>
       <c r="O7">
         <f>D16</f>
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="P7">
         <f>D17/1000</f>
@@ -1654,19 +1519,19 @@
       </c>
       <c r="Q7">
         <f>F15</f>
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="R7">
         <f>F16</f>
         <v>107</v>
       </c>
       <c r="S7">
-        <f>E15</f>
-        <v>52</v>
+        <f>E15/H15*100</f>
+        <v>111.90476190476191</v>
       </c>
       <c r="T7">
-        <f>G15</f>
-        <v>37</v>
+        <f>G15/H15*100</f>
+        <v>92.857142857142861</v>
       </c>
       <c r="U7">
         <f>H15</f>
@@ -1674,32 +1539,32 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="3" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="24">
         <v>512</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="15"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="30"/>
       <c r="M8">
         <f>B18</f>
         <v>49</v>
       </c>
       <c r="N8">
         <f>D18</f>
-        <v>627</v>
+        <v>449</v>
       </c>
       <c r="O8">
         <f>D19</f>
-        <v>354</v>
+        <v>248</v>
       </c>
       <c r="P8">
         <f>D20/1000</f>
@@ -1707,19 +1572,19 @@
       </c>
       <c r="Q8">
         <f>F18</f>
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="R8">
         <f>F19</f>
         <v>107</v>
       </c>
       <c r="S8">
-        <f>E18</f>
-        <v>73</v>
+        <f>E18/H18*100</f>
+        <v>120.68965517241379</v>
       </c>
       <c r="T8">
-        <f>G18</f>
-        <v>50</v>
+        <f>G18/H18*100</f>
+        <v>86.206896551724128</v>
       </c>
       <c r="U8">
         <f>H18</f>
@@ -1727,38 +1592,38 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="5">
         <v>16</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5">
-        <v>227</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="D9" s="4">
+        <v>183</v>
+      </c>
+      <c r="E9" s="4">
+        <v>18</v>
+      </c>
+      <c r="F9" s="4">
+        <v>108</v>
+      </c>
+      <c r="G9" s="4">
         <v>19</v>
       </c>
-      <c r="F9" s="5">
-        <v>89</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <v>19</v>
       </c>
-      <c r="H9" s="10">
-        <v>19</v>
-      </c>
-      <c r="I9" s="10">
+      <c r="I9" s="5">
         <v>206</v>
       </c>
-      <c r="J9" s="10">
-        <v>96</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>32</v>
+      <c r="J9" s="5">
+        <v>118</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="M9">
         <f>B21</f>
@@ -1766,11 +1631,11 @@
       </c>
       <c r="N9">
         <f>D21</f>
-        <v>649</v>
+        <v>579</v>
       </c>
       <c r="O9">
         <f>D22</f>
-        <v>445</v>
+        <v>307</v>
       </c>
       <c r="P9">
         <f>D23/1000</f>
@@ -1778,19 +1643,19 @@
       </c>
       <c r="Q9">
         <f>F21</f>
-        <v>100</v>
+        <v>181</v>
       </c>
       <c r="R9">
         <f>F22</f>
         <v>108</v>
       </c>
       <c r="S9">
-        <f>E21</f>
-        <v>111</v>
+        <f>E21/H21*100</f>
+        <v>136.7816091954023</v>
       </c>
       <c r="T9">
-        <f>G21</f>
-        <v>78</v>
+        <f>G21/H21*100</f>
+        <v>93.103448275862064</v>
       </c>
       <c r="U9">
         <f>H21</f>
@@ -1798,34 +1663,34 @@
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="7"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="1">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
         <v>105</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="14"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="9"/>
       <c r="M10">
         <f>B24</f>
         <v>81</v>
       </c>
       <c r="N10">
         <f>D24</f>
-        <v>812</v>
+        <v>771</v>
       </c>
       <c r="O10">
         <f>D25</f>
-        <v>551</v>
+        <v>379</v>
       </c>
       <c r="P10">
         <f>D26/1000</f>
@@ -1833,19 +1698,19 @@
       </c>
       <c r="Q10">
         <f>F24</f>
-        <v>100</v>
+        <v>222</v>
       </c>
       <c r="R10">
         <f>F25</f>
         <v>108</v>
       </c>
       <c r="S10">
-        <f>E24</f>
-        <v>167</v>
+        <f>E24/H24*100</f>
+        <v>158.40707964601771</v>
       </c>
       <c r="T10">
-        <f>G24</f>
-        <v>121</v>
+        <f>G24/H24*100</f>
+        <v>107.07964601769913</v>
       </c>
       <c r="U10">
         <f>H24</f>
@@ -1853,391 +1718,397 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3">
-        <v>1024</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="15"/>
+      <c r="D11" s="2">
+        <v>512</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="5">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="5">
-        <v>340</v>
-      </c>
-      <c r="E12" s="5">
-        <v>26</v>
-      </c>
-      <c r="F12" s="5">
-        <v>98</v>
-      </c>
-      <c r="G12" s="5">
-        <v>22</v>
-      </c>
-      <c r="H12" s="10">
+      <c r="D12" s="4">
+        <v>250</v>
+      </c>
+      <c r="E12" s="4">
+        <v>28</v>
+      </c>
+      <c r="F12" s="4">
+        <v>121</v>
+      </c>
+      <c r="G12" s="4">
+        <v>23</v>
+      </c>
+      <c r="H12" s="5">
         <v>27</v>
       </c>
-      <c r="I12" s="10">
-        <v>154</v>
-      </c>
-      <c r="J12" s="10">
-        <v>96</v>
-      </c>
-      <c r="K12" s="13"/>
+      <c r="I12" s="5">
+        <v>196</v>
+      </c>
+      <c r="J12" s="5">
+        <v>115</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="7"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="1">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
         <v>106</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="14"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="3" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>1024</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="15"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="5">
         <v>36</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="5">
-        <v>445</v>
-      </c>
-      <c r="E15" s="5">
-        <v>52</v>
-      </c>
-      <c r="F15" s="5">
-        <v>99</v>
-      </c>
-      <c r="G15" s="5">
-        <v>37</v>
-      </c>
-      <c r="H15" s="10">
+      <c r="D15" s="4">
+        <v>347</v>
+      </c>
+      <c r="E15" s="4">
+        <v>47</v>
+      </c>
+      <c r="F15" s="4">
+        <v>138</v>
+      </c>
+      <c r="G15" s="4">
+        <v>39</v>
+      </c>
+      <c r="H15" s="5">
         <v>42</v>
       </c>
-      <c r="I15" s="10">
-        <v>138</v>
-      </c>
-      <c r="J15" s="10">
-        <v>101</v>
-      </c>
-      <c r="K15" s="13"/>
+      <c r="I15" s="5">
+        <v>184</v>
+      </c>
+      <c r="J15" s="5">
+        <v>110</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="7"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="1">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
         <v>107</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="14"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>2048</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="15"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="5">
         <v>49</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="5">
-        <v>627</v>
-      </c>
-      <c r="E18" s="5">
-        <v>73</v>
-      </c>
-      <c r="F18" s="5">
-        <v>99</v>
-      </c>
-      <c r="G18" s="5">
+      <c r="D18" s="4">
+        <v>449</v>
+      </c>
+      <c r="E18" s="4">
+        <v>70</v>
+      </c>
+      <c r="F18" s="4">
+        <v>149</v>
+      </c>
+      <c r="G18" s="4">
         <v>50</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="5">
         <v>58</v>
       </c>
-      <c r="I18" s="10">
-        <v>128</v>
-      </c>
-      <c r="J18" s="10">
-        <v>100</v>
-      </c>
-      <c r="K18" s="13"/>
+      <c r="I18" s="5">
+        <v>175</v>
+      </c>
+      <c r="J18" s="5">
+        <v>110</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="7"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="1">
-        <v>354</v>
+        <v>248</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1">
         <v>107</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="14"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="3" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>2048</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="15"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="5">
         <v>64</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="5">
-        <v>649</v>
-      </c>
-      <c r="E21" s="5">
-        <v>111</v>
-      </c>
-      <c r="F21" s="5">
-        <v>100</v>
-      </c>
-      <c r="G21" s="5">
-        <v>78</v>
-      </c>
-      <c r="H21" s="10">
+      <c r="D21" s="4">
+        <v>579</v>
+      </c>
+      <c r="E21" s="4">
+        <v>119</v>
+      </c>
+      <c r="F21" s="4">
+        <v>181</v>
+      </c>
+      <c r="G21" s="4">
+        <v>81</v>
+      </c>
+      <c r="H21" s="5">
         <v>87</v>
       </c>
-      <c r="I21" s="10">
-        <v>133</v>
-      </c>
-      <c r="J21" s="10">
-        <v>101</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>22</v>
+      <c r="I21" s="5">
+        <v>156</v>
+      </c>
+      <c r="J21" s="5">
+        <v>106</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="7"/>
-      <c r="B22" s="11"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="1">
-        <v>445</v>
+        <v>307</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1">
         <v>108</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="14"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="3" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>2048</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="15"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="5">
         <v>81</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="5">
-        <v>812</v>
-      </c>
-      <c r="E24" s="5">
-        <v>167</v>
-      </c>
-      <c r="F24" s="5">
-        <v>100</v>
-      </c>
-      <c r="G24" s="5">
+      <c r="D24" s="4">
+        <v>771</v>
+      </c>
+      <c r="E24" s="4">
+        <v>179</v>
+      </c>
+      <c r="F24" s="4">
+        <v>222</v>
+      </c>
+      <c r="G24" s="4">
         <v>121</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="5">
         <v>113</v>
       </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="13" t="s">
-        <v>23</v>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="7"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="1">
-        <v>551</v>
+        <v>379</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1">
         <v>108</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="14"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="3" t="s">
+      <c r="A26" s="13"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>4096</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="15"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="5">
         <v>100</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="10">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="5">
         <v>157</v>
       </c>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="13"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="7"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
@@ -2245,28 +2116,66 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="14"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="9"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="3" t="s">
+      <c r="A29" s="13"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="15"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="K21:K23"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="K24:K26"/>
     <mergeCell ref="K27:K29"/>
@@ -2283,47 +2192,8 @@
     <mergeCell ref="H27:H29"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="K6:K8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="K21:K23"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
New results for the single clocked network adapter.
</commit_message>
<xml_diff>
--- a/noc/results/results.xlsx
+++ b/noc/results/results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="18870" windowHeight="10185" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="18870" windowHeight="10185" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram1" sheetId="4" r:id="rId1"/>
-    <sheet name="Ark1" sheetId="1" r:id="rId2"/>
-    <sheet name="Ark2" sheetId="2" r:id="rId3"/>
+    <sheet name="Dual clocked" sheetId="1" r:id="rId2"/>
+    <sheet name="Single clocked" sheetId="2" r:id="rId3"/>
     <sheet name="Ark3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="34">
   <si>
     <t>Resources pr. tile</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Did not fit in the Cyclon 2 chip</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>RX and TX ram implementet in LUT and Registers: old</t>
   </si>
 </sst>
 </file>
@@ -256,6 +262,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -274,6 +284,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -286,45 +323,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -351,7 +357,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$M$3:$M$10</c:f>
+              <c:f>'Dual clocked'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -384,7 +390,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ark1'!$N$3:$N$10</c:f>
+              <c:f>'Dual clocked'!$N$3:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -425,7 +431,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$M$3:$M$10</c:f>
+              <c:f>'Dual clocked'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -458,7 +464,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ark1'!$O$3:$O$10</c:f>
+              <c:f>'Dual clocked'!$O$3:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -499,7 +505,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$M$3:$M$10</c:f>
+              <c:f>'Dual clocked'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -532,7 +538,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ark1'!$P$3:$P$10</c:f>
+              <c:f>'Dual clocked'!$P$3:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -573,7 +579,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$M$3:$M$10</c:f>
+              <c:f>'Dual clocked'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -606,7 +612,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ark1'!$Q$3:$Q$10</c:f>
+              <c:f>'Dual clocked'!$Q$3:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -647,7 +653,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$M$3:$M$10</c:f>
+              <c:f>'Dual clocked'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -680,7 +686,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ark1'!$R$3:$R$10</c:f>
+              <c:f>'Dual clocked'!$R$3:$R$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -721,7 +727,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$M$3:$M$10</c:f>
+              <c:f>'Dual clocked'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -754,7 +760,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ark1'!$U$3:$U$10</c:f>
+              <c:f>'Dual clocked'!$U$3:$U$10</c:f>
               <c:numCache>
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="8"/>
@@ -787,23 +793,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="87264640"/>
-        <c:axId val="87274624"/>
+        <c:axId val="63713280"/>
+        <c:axId val="63714816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87264640"/>
+        <c:axId val="63713280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="Standard" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87274624"/>
+        <c:crossAx val="63714816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87274624"/>
+        <c:axId val="63714816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +817,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="Standard" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87264640"/>
+        <c:crossAx val="63713280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
@@ -820,7 +826,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -831,7 +836,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1152,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1236,34 +1241,34 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="15">
         <v>4</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="5">
         <v>86</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="5">
         <v>4</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="5">
         <v>44</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="5">
         <v>4</v>
       </c>
       <c r="H3" s="15">
         <v>5</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="16">
         <v>207</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="16">
         <v>103</v>
       </c>
       <c r="K3" s="18" t="s">
@@ -1307,23 +1312,23 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="19"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="20" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="6">
         <v>64</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6">
         <v>100</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="21"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="19"/>
       <c r="M4">
         <f>B6</f>
         <v>9</v>
@@ -1362,21 +1367,21 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="7">
         <v>256</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="25"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="20"/>
       <c r="M5">
         <f>B9</f>
         <v>16</v>
@@ -1415,25 +1420,25 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="15">
         <v>9</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="8">
         <v>159</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="8">
         <v>6</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="8">
         <v>71</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="8">
         <v>7</v>
       </c>
       <c r="H6" s="15">
@@ -1445,7 +1450,7 @@
       <c r="J6" s="15">
         <v>97</v>
       </c>
-      <c r="K6" s="28"/>
+      <c r="K6" s="21"/>
       <c r="M6">
         <f>B12</f>
         <v>25</v>
@@ -1484,23 +1489,23 @@
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="19"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="20" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="6">
         <v>104</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
         <v>103</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="29"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="22"/>
       <c r="M7">
         <f>B15</f>
         <v>36</v>
@@ -1539,21 +1544,21 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="7">
         <v>512</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="30"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="23"/>
       <c r="M8">
         <f>B18</f>
         <v>49</v>
@@ -1592,10 +1597,10 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1613,16 +1618,16 @@
       <c r="G9" s="4">
         <v>19</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="9">
         <v>19</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="9">
         <v>206</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="9">
         <v>118</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="12" t="s">
         <v>30</v>
       </c>
       <c r="M9">
@@ -1663,8 +1668,8 @@
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="12"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1676,10 +1681,10 @@
         <v>105</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="9"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="13"/>
       <c r="M10">
         <f>B24</f>
         <v>81</v>
@@ -1718,8 +1723,8 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A11" s="13"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1729,16 +1734,16 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="9">
         <v>25</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1756,22 +1761,22 @@
       <c r="G12" s="4">
         <v>23</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="9">
         <v>27</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="9">
         <v>196</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="9">
         <v>115</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="12"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1783,14 +1788,14 @@
         <v>106</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="9"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1800,16 +1805,16 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="9">
         <v>36</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1827,22 +1832,22 @@
       <c r="G15" s="4">
         <v>39</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="9">
         <v>42</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="9">
         <v>184</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="9">
         <v>110</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="12"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1854,14 +1859,14 @@
         <v>107</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="9"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1871,16 +1876,16 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="9">
         <v>49</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1898,22 +1903,22 @@
       <c r="G18" s="4">
         <v>50</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="9">
         <v>58</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="9">
         <v>175</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="9">
         <v>110</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="12"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1925,14 +1930,14 @@
         <v>107</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="9"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="13"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
@@ -1942,16 +1947,16 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="9">
         <v>64</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1969,22 +1974,22 @@
       <c r="G21" s="4">
         <v>81</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="9">
         <v>87</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="9">
         <v>156</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="9">
         <v>106</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="12"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1996,14 +2001,14 @@
         <v>108</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="9"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="13"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
@@ -2013,16 +2018,16 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="10"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="9">
         <v>81</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -2040,18 +2045,18 @@
       <c r="G24" s="4">
         <v>121</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="9">
         <v>113</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="8" t="s">
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="12"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
@@ -2063,14 +2068,14 @@
         <v>108</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="9"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="13"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A26" s="13"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="2" t="s">
         <v>15</v>
       </c>
@@ -2080,16 +2085,16 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="10"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="14"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="9">
         <v>100</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -2099,16 +2104,16 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="5">
+      <c r="H27" s="9">
         <v>157</v>
       </c>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="8"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="12"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
@@ -2116,14 +2121,14 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="9"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="13"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A29" s="13"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
@@ -2131,10 +2136,10 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="10"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="54">
@@ -2199,12 +2204,969 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="15">
+        <v>5</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="18"/>
+      <c r="L3">
+        <f>B3</f>
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <f>D3</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>D4</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>D5/1000</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>F3</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>F4</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>E3/H3*100</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f>G3/H3*100</f>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f>H3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="28"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="19"/>
+      <c r="L4">
+        <f>B6</f>
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <f>D6</f>
+        <v>288</v>
+      </c>
+      <c r="N4">
+        <f>D7</f>
+        <v>328</v>
+      </c>
+      <c r="O4">
+        <f>D8/1000</f>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f>F6</f>
+        <v>117</v>
+      </c>
+      <c r="Q4">
+        <f>F7</f>
+        <v>102</v>
+      </c>
+      <c r="R4">
+        <f>E6/H6*100</f>
+        <v>160</v>
+      </c>
+      <c r="S4">
+        <f>G6/H6*100</f>
+        <v>120</v>
+      </c>
+      <c r="T4">
+        <f>H6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A5" s="29"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="20"/>
+      <c r="L5">
+        <f>B9</f>
+        <v>16</v>
+      </c>
+      <c r="M5">
+        <f>D9</f>
+        <v>179</v>
+      </c>
+      <c r="N5">
+        <f>D10</f>
+        <v>55</v>
+      </c>
+      <c r="O5">
+        <f>D11/1000</f>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="P5">
+        <f>F9</f>
+        <v>115</v>
+      </c>
+      <c r="Q5">
+        <f>F10</f>
+        <v>106</v>
+      </c>
+      <c r="R5">
+        <f>E9/H9*100</f>
+        <v>68.421052631578945</v>
+      </c>
+      <c r="S5">
+        <f>G9/H9*100</f>
+        <v>147.36842105263156</v>
+      </c>
+      <c r="T5">
+        <f>H9</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="15">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8">
+        <v>288</v>
+      </c>
+      <c r="E6" s="8">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8">
+        <v>117</v>
+      </c>
+      <c r="G6" s="8">
+        <v>12</v>
+      </c>
+      <c r="H6" s="15">
+        <v>10</v>
+      </c>
+      <c r="I6" s="15">
+        <v>103.7</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6">
+        <f>B12</f>
+        <v>25</v>
+      </c>
+      <c r="M6">
+        <f>D12</f>
+        <v>191</v>
+      </c>
+      <c r="N6">
+        <f>D13</f>
+        <v>64</v>
+      </c>
+      <c r="O6">
+        <f>D14/1000</f>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="P6">
+        <f>F12</f>
+        <v>131</v>
+      </c>
+      <c r="Q6">
+        <f>F13</f>
+        <v>107</v>
+      </c>
+      <c r="R6">
+        <f>E12/H12*100</f>
+        <v>85.18518518518519</v>
+      </c>
+      <c r="S6">
+        <f>G12/H12*100</f>
+        <v>140.74074074074073</v>
+      </c>
+      <c r="T6">
+        <f>H12</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="28"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6">
+        <v>328</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
+        <v>102</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="22"/>
+      <c r="L7">
+        <f>B15</f>
+        <v>36</v>
+      </c>
+      <c r="M7">
+        <f>D15</f>
+        <v>230</v>
+      </c>
+      <c r="N7">
+        <f>D16</f>
+        <v>76</v>
+      </c>
+      <c r="O7">
+        <f>D17/1000</f>
+        <v>2.048</v>
+      </c>
+      <c r="P7">
+        <f>F15</f>
+        <v>152</v>
+      </c>
+      <c r="Q7">
+        <f>F16</f>
+        <v>110</v>
+      </c>
+      <c r="R7">
+        <f>E15/H15*100</f>
+        <v>92.857142857142861</v>
+      </c>
+      <c r="S7">
+        <f>G15/H15*100</f>
+        <v>150</v>
+      </c>
+      <c r="T7">
+        <f>H15</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A8" s="29"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="23"/>
+      <c r="L8">
+        <f>B18</f>
+        <v>49</v>
+      </c>
+      <c r="M8">
+        <f>D18</f>
+        <v>262</v>
+      </c>
+      <c r="N8">
+        <f>D19</f>
+        <v>89</v>
+      </c>
+      <c r="O8">
+        <f>D20/1000</f>
+        <v>2.048</v>
+      </c>
+      <c r="P8">
+        <f>F18</f>
+        <v>131</v>
+      </c>
+      <c r="Q8">
+        <f>F19</f>
+        <v>108</v>
+      </c>
+      <c r="R8">
+        <f>E18/H18*100</f>
+        <v>79.310344827586206</v>
+      </c>
+      <c r="S8">
+        <f>G18/H18*100</f>
+        <v>134.48275862068965</v>
+      </c>
+      <c r="T8">
+        <f>H18</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="9">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4">
+        <v>179</v>
+      </c>
+      <c r="E9" s="4">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4">
+        <v>115</v>
+      </c>
+      <c r="G9" s="4">
+        <v>28</v>
+      </c>
+      <c r="H9" s="9">
+        <v>19</v>
+      </c>
+      <c r="I9" s="9">
+        <v>105</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9">
+        <f>B21</f>
+        <v>64</v>
+      </c>
+      <c r="M9">
+        <f>D21</f>
+        <v>297</v>
+      </c>
+      <c r="N9">
+        <f>D22</f>
+        <v>105</v>
+      </c>
+      <c r="O9">
+        <f>D23/1000</f>
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="P9">
+        <f>F21</f>
+        <v>170</v>
+      </c>
+      <c r="Q9">
+        <f>F22</f>
+        <v>112</v>
+      </c>
+      <c r="R9">
+        <f>E21/H21*100</f>
+        <v>81.609195402298852</v>
+      </c>
+      <c r="S9">
+        <f>G21/H21*100</f>
+        <v>145.97701149425288</v>
+      </c>
+      <c r="T9">
+        <f>H21</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="25"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1">
+        <v>55</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>106</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="13"/>
+      <c r="L10">
+        <f>B24</f>
+        <v>81</v>
+      </c>
+      <c r="M10">
+        <f>D24</f>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f>D25</f>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>D26/1000</f>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f>F24</f>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f>F25</f>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f>E24/H24*100</f>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f>G24/H24*100</f>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f>H24</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A11" s="26"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2">
+        <v>512</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="4">
+        <v>191</v>
+      </c>
+      <c r="E12" s="4">
+        <v>23</v>
+      </c>
+      <c r="F12" s="4">
+        <v>131</v>
+      </c>
+      <c r="G12" s="4">
+        <v>38</v>
+      </c>
+      <c r="H12" s="9">
+        <v>27</v>
+      </c>
+      <c r="I12" s="9">
+        <v>103.6</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="25"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1">
+        <v>64</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <v>107</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A14" s="26"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2">
+        <v>512</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4">
+        <v>230</v>
+      </c>
+      <c r="E15" s="4">
+        <v>39</v>
+      </c>
+      <c r="F15" s="4">
+        <v>152</v>
+      </c>
+      <c r="G15" s="4">
+        <v>63</v>
+      </c>
+      <c r="H15" s="9">
+        <v>42</v>
+      </c>
+      <c r="I15" s="9">
+        <v>104.3</v>
+      </c>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="25"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1">
+        <v>76</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>110</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A17" s="26"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2048</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="9">
+        <v>49</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4">
+        <v>262</v>
+      </c>
+      <c r="E18" s="4">
+        <v>46</v>
+      </c>
+      <c r="F18" s="4">
+        <v>131</v>
+      </c>
+      <c r="G18" s="4">
+        <v>78</v>
+      </c>
+      <c r="H18" s="9">
+        <v>58</v>
+      </c>
+      <c r="I18" s="9">
+        <v>106</v>
+      </c>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="25"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1">
+        <v>89</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
+        <v>108</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A20" s="26"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2048</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="9">
+        <v>64</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4">
+        <v>297</v>
+      </c>
+      <c r="E21" s="4">
+        <v>71</v>
+      </c>
+      <c r="F21" s="4">
+        <v>170</v>
+      </c>
+      <c r="G21" s="4">
+        <v>127</v>
+      </c>
+      <c r="H21" s="9">
+        <v>87</v>
+      </c>
+      <c r="I21" s="9">
+        <v>104.8</v>
+      </c>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="25"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1">
+        <v>105</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <v>112</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A23" s="26"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="2">
+        <v>4096</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="9">
+        <v>81</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="9">
+        <v>113</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="25"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A26" s="26"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="9">
+        <v>100</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="9">
+        <v>157</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="25"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A29" s="26"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="45">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="J27:J29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>